<commit_message>
Frequent Radiosoundings Site 2
</commit_message>
<xml_diff>
--- a/BLLAST/Tethersonde-SUMO Description.xlsx
+++ b/BLLAST/Tethersonde-SUMO Description.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="4660" windowWidth="20120" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="27180" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tethersonde" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="67">
   <si>
     <t>Year</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>End Long</t>
+  </si>
+  <si>
+    <t>Latitude:</t>
+  </si>
+  <si>
+    <t>Longitude:</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -596,8 +602,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="257">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1187,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
@@ -2402,18 +2408,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1">
+        <v>43.133099999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2">
+        <v>0.3669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2421,7 +2443,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="4" customFormat="1">
+    <row r="4" spans="1:5" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2429,7 +2451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="4" customFormat="1">
+    <row r="5" spans="1:5" s="4" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>